<commit_message>
GuideQuestTable 에 viewInBattle|Bool 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Quest.xlsx
+++ b/Excel/Quest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D3BA4A-BE60-45C1-A4EF-94F0D572B2FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB659B0-49AF-4DE5-B3BF-2E4AA0B136D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D81F9E31-8774-41AE-8DB9-A825D81F47C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D81F9E31-8774-41AE-8DB9-A825D81F47C2}"/>
   </bookViews>
   <sheets>
     <sheet name="SubQuestTable" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>type|String</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>SubQuestShortDesc_8</t>
+  </si>
+  <si>
+    <t>viewInBattle|Bool</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75EAC42-57D5-4465-95F3-77B68A2F422D}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -765,19 +768,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8211884E-E6DD-41A3-AFCA-197A318D2388}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="19.25" customWidth="1"/>
-    <col min="5" max="5" width="13.75" customWidth="1"/>
-    <col min="6" max="6" width="10.375" customWidth="1"/>
-    <col min="11" max="11" width="24.125" customWidth="1"/>
+    <col min="6" max="6" width="13.75" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="12" max="12" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -791,28 +794,31 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -825,26 +831,29 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>38</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>500</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -857,26 +866,29 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>40</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
       </c>
       <c r="J3">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -889,26 +901,29 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>37</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>41</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>8</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>4</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -921,26 +936,29 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>37</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>42</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>2</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>3</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -953,26 +971,29 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>43</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>3</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -985,23 +1006,26 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>44</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1014,19 +1038,22 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>45</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
       <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
         <v>0</v>
       </c>
     </row>

</xml_diff>